<commit_message>
#1791 - Asset Folder Creator to support non-string cell types (ie. Numeric)
</commit_message>
<xml_diff>
--- a/bundle/src/test/resources/com/adobe/acs/commons/mcp/impl/processes/asset-folder-creator.xlsx
+++ b/bundle/src/test/resources/com/adobe/acs/commons/mcp/impl/processes/asset-folder-creator.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dgonzale/Code/acs/acs-aem-commons/bundle/src/test/resources/com/adobe/acs/commons/mcp/impl/processes/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE24DB0-8C4B-4F4F-BC0A-DB692F8AC1CB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1180" windowWidth="24420" windowHeight="14820" tabRatio="500"/>
+    <workbookView xWindow="1180" yWindow="1180" windowWidth="24420" windowHeight="14820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -65,13 +66,13 @@
     <t>Michigan {{ mi }}</t>
   </si>
   <si>
-    <t>Massachusettes {{ ma }}</t>
+    <t>Massachusetts {{ ma }}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -120,6 +121,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -387,11 +391,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -499,6 +503,17 @@
         <v>10</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2019</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
#1791 - Asset Folder Creator to support non-string cell types (ie. Nu… (#1792)
* #1791 - Asset Folder Creator to support non-string cell types (ie. Numeric)
</commit_message>
<xml_diff>
--- a/bundle/src/test/resources/com/adobe/acs/commons/mcp/impl/processes/asset-folder-creator.xlsx
+++ b/bundle/src/test/resources/com/adobe/acs/commons/mcp/impl/processes/asset-folder-creator.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dgonzale/Code/acs/acs-aem-commons/bundle/src/test/resources/com/adobe/acs/commons/mcp/impl/processes/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE24DB0-8C4B-4F4F-BC0A-DB692F8AC1CB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1180" windowWidth="24420" windowHeight="14820" tabRatio="500"/>
+    <workbookView xWindow="1180" yWindow="1180" windowWidth="24420" windowHeight="14820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -65,13 +66,13 @@
     <t>Michigan {{ mi }}</t>
   </si>
   <si>
-    <t>Massachusettes {{ ma }}</t>
+    <t>Massachusetts {{ ma }}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -120,6 +121,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -387,11 +391,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -499,6 +503,17 @@
         <v>10</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2019</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>